<commit_message>
infer age distribution of new entrants based on low yos actives
</commit_message>
<xml_diff>
--- a/RunControl(6).xlsx
+++ b/RunControl(6).xlsx
@@ -1985,10 +1985,10 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>20</v>

</xml_diff>

<commit_message>
add a more flexible way to create investment returns.
</commit_message>
<xml_diff>
--- a/RunControl(6).xlsx
+++ b/RunControl(6).xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
     <sheet name="RunControl" sheetId="3" r:id="rId3"/>
-    <sheet name="GlobalParams" sheetId="4" r:id="rId4"/>
-    <sheet name="DropDowns" sheetId="5" r:id="rId5"/>
+    <sheet name="Returns" sheetId="6" r:id="rId4"/>
+    <sheet name="GlobalParams" sheetId="4" r:id="rId5"/>
+    <sheet name="DropDowns" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$7</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="164">
   <si>
     <t>Sheet #</t>
   </si>
@@ -403,9 +405,6 @@
     <t>average2</t>
   </si>
   <si>
-    <t>another description</t>
-  </si>
-  <si>
     <t>EAN.CD</t>
   </si>
   <si>
@@ -512,6 +511,15 @@
   </si>
   <si>
     <t>as found in the Winklevoss book</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>return_type</t>
+  </si>
+  <si>
+    <t>internal</t>
   </si>
 </sst>
 </file>
@@ -645,7 +653,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -677,7 +685,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,21 +709,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1202,13 +1211,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AM8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1221,23 +1230,25 @@
     <col min="13" max="14" width="21.44140625"/>
     <col min="15" max="15" width="24.5546875"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="32" width="12.6640625"/>
-    <col min="33" max="35" width="27.109375"/>
-    <col min="36" max="36" width="20.6640625"/>
-    <col min="37" max="37" width="26.88671875"/>
-    <col min="38" max="38" width="16"/>
-    <col min="39" max="1025" width="8.5546875"/>
+    <col min="17" max="21" width="12.6640625"/>
+    <col min="22" max="22" width="11.109375" customWidth="1"/>
+    <col min="23" max="33" width="12.6640625"/>
+    <col min="34" max="36" width="27.109375"/>
+    <col min="37" max="37" width="20.6640625"/>
+    <col min="38" max="38" width="26.88671875"/>
+    <col min="39" max="39" width="16"/>
+    <col min="40" max="1026" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="AB1" s="1" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-    </row>
-    <row r="2" spans="1:38" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1289,27 +1300,27 @@
       <c r="U2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
-      <c r="AL2" s="4" t="s">
+      <c r="AK2" s="6"/>
+      <c r="AM2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1334,98 +1345,99 @@
       <c r="O3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AE3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AH3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:38" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:39" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20" t="s">
+      <c r="G4" s="24"/>
+      <c r="H4" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="20" t="s">
+      <c r="K4" s="20"/>
+      <c r="L4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21" t="s">
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="22" t="s">
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="22"/>
-      <c r="X4" s="7" t="s">
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Y4" s="17" t="s">
+      <c r="Z4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="Z4" s="17"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="24" t="s">
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="22" t="s">
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="23" t="s">
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="23"/>
-    </row>
-    <row r="5" spans="1:38" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+    </row>
+    <row r="5" spans="1:39" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
@@ -1490,58 +1502,61 @@
         <v>92</v>
       </c>
       <c r="V5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="AF5" s="9" t="s">
+      <c r="AG5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AG5" s="9" t="s">
+      <c r="AH5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AI5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AM5" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1604,73 +1619,94 @@
         <v>0.01</v>
       </c>
       <c r="U6" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="W6" s="12">
         <v>0.08</v>
       </c>
-      <c r="V6" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="W6" s="12">
+      <c r="X6" s="12">
         <v>0.12</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>115</v>
       </c>
-      <c r="Y6" s="2" t="s">
+      <c r="Z6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Z6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>3</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AC6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AC6" s="14">
+      <c r="AD6" s="14">
         <v>0.25</v>
       </c>
-      <c r="AD6" s="14">
+      <c r="AE6" s="14">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AE6" s="14">
+      <c r="AF6" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>200</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AH6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>120</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>10</v>
       </c>
-      <c r="AJ6" s="2" t="s">
+      <c r="AK6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>200</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C7" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="D7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
       <c r="J7" s="12">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K7" s="13" t="b">
         <v>1</v>
@@ -1703,72 +1739,85 @@
         <v>0.01</v>
       </c>
       <c r="U7" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V7" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="W7" s="12">
         <v>0.08</v>
       </c>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" t="s">
+      <c r="X7" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y7" t="s">
         <v>115</v>
       </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="AA7" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>3</v>
       </c>
-      <c r="AB7" s="2" t="s">
+      <c r="AC7" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AC7" s="14">
+      <c r="AD7" s="14">
         <v>0.25</v>
       </c>
-      <c r="AD7" s="14">
+      <c r="AE7" s="14">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AE7" s="14">
+      <c r="AF7" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>200</v>
       </c>
-      <c r="AG7" s="2" t="s">
+      <c r="AH7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AJ7" s="2" t="s">
+      <c r="AI7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ7">
+        <v>10</v>
+      </c>
+      <c r="AK7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>200</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="J8" s="12">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K8" s="13" t="b">
         <v>1</v>
       </c>
       <c r="L8" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N8">
         <v>65</v>
@@ -1796,83 +1845,84 @@
       </c>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
-      <c r="X8" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y8" s="2" t="s">
+      <c r="X8" s="12"/>
+      <c r="Y8" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>3</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AC8" s="14">
+      <c r="AD8" s="14">
         <v>0.25</v>
       </c>
-      <c r="AD8" s="14">
+      <c r="AE8" s="14">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AF8" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>200</v>
       </c>
-      <c r="AG8" s="2" t="s">
+      <c r="AH8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AK8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>200</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AH4:AL4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AE4"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AM4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="V4:X4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG8">
+  <dataValidations count="18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH8">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK8">
       <formula1>"MA,AL"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA8">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z8">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB6:AB8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC8">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C8 K6:K8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K8 C6:C8">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1880,7 +1930,7 @@
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P8 T6:T8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T8 P6:P8">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
@@ -1888,50 +1938,161 @@
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S8 U6:V8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V8 W6:W8 U6:U8 S6:S8">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AA6:AA8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB8">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AC6:AD8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE8">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AE6:AE8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF8">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="W6:W8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X8">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AI6:AI8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AJ6:AJ8">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL8">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL8">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM8">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V7"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="V7" r:id="rId1" location="Returns!A1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="D4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="12">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="C4:C7">
+      <formula1>0</formula1>
+      <formula2>0.75</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B7">
+      <formula1>0</formula1>
+      <formula2>0.2</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>GlobalParams!A3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,38 +2102,38 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B3">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1996,11 +2157,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2014,7 +2175,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2024,15 +2185,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>137</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2045,23 +2206,23 @@
         <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
         <v>141</v>
-      </c>
-      <c r="C9" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2074,23 +2235,23 @@
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
         <v>144</v>
-      </c>
-      <c r="C13" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
         <v>146</v>
-      </c>
-      <c r="C14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2103,15 +2264,15 @@
         <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" t="s">
         <v>149</v>
-      </c>
-      <c r="C18" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2124,15 +2285,15 @@
         <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
         <v>149</v>
-      </c>
-      <c r="C22" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2145,15 +2306,15 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
         <v>149</v>
-      </c>
-      <c r="C26" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2166,15 +2327,15 @@
         <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" t="s">
         <v>149</v>
-      </c>
-      <c r="C30" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2187,15 +2348,15 @@
         <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" t="s">
         <v>152</v>
-      </c>
-      <c r="C34" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2208,31 +2369,31 @@
         <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
         <v>155</v>
-      </c>
-      <c r="C38" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" t="s">
         <v>157</v>
-      </c>
-      <c r="C39" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
         <v>159</v>
-      </c>
-      <c r="C40" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2245,7 +2406,7 @@
         <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user can control the ERC paid in a specified period
</commit_message>
<xml_diff>
--- a/RunControl(6).xlsx
+++ b/RunControl(6).xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
     <sheet name="RunControl" sheetId="3" r:id="rId3"/>
     <sheet name="Returns" sheetId="6" r:id="rId4"/>
-    <sheet name="GlobalParams" sheetId="4" r:id="rId5"/>
-    <sheet name="DropDowns" sheetId="5" r:id="rId6"/>
+    <sheet name="Contributions" sheetId="7" r:id="rId5"/>
+    <sheet name="GlobalParams" sheetId="4" r:id="rId6"/>
+    <sheet name="DropDowns" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$6</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="167">
   <si>
     <t>Sheet #</t>
   </si>
@@ -396,12 +397,6 @@
     <t>AL</t>
   </si>
   <si>
-    <t>underfunded1</t>
-  </si>
-  <si>
-    <t>different description</t>
-  </si>
-  <si>
     <t>average2</t>
   </si>
   <si>
@@ -520,6 +515,21 @@
   </si>
   <si>
     <t>internal</t>
+  </si>
+  <si>
+    <t>average3</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>pct_ADC</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>exCon</t>
   </si>
 </sst>
 </file>
@@ -653,7 +663,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,6 +695,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -710,6 +723,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1211,13 +1229,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM8"/>
+  <dimension ref="A1:AN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="U8" sqref="U8"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,23 +1250,25 @@
     <col min="16" max="16" width="16"/>
     <col min="17" max="21" width="12.6640625"/>
     <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="23" max="33" width="12.6640625"/>
-    <col min="34" max="36" width="27.109375"/>
-    <col min="37" max="37" width="20.6640625"/>
-    <col min="38" max="38" width="26.88671875"/>
-    <col min="39" max="39" width="16"/>
-    <col min="40" max="1026" width="8.5546875"/>
+    <col min="23" max="32" width="12.6640625"/>
+    <col min="34" max="34" width="12.6640625"/>
+    <col min="35" max="37" width="27.109375"/>
+    <col min="38" max="38" width="20.6640625"/>
+    <col min="39" max="39" width="26.88671875"/>
+    <col min="40" max="40" width="16"/>
+    <col min="41" max="1027" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
-    </row>
-    <row r="2" spans="1:39" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" spans="1:40" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1309,18 +1329,18 @@
       <c r="AE2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="6"/>
-      <c r="AM2" s="4" t="s">
+      <c r="AL2" s="6"/>
+      <c r="AN2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1354,90 +1374,91 @@
       <c r="AE3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AI3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:40" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="19" t="s">
+      <c r="G4" s="25"/>
+      <c r="H4" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20" t="s">
+      <c r="I4" s="20"/>
+      <c r="J4" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="19" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="20" t="s">
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="17" t="s">
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
       <c r="Y4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="22" t="s">
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="17" t="s">
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="18" t="s">
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="AJ4" s="18"/>
-      <c r="AK4" s="18"/>
-      <c r="AL4" s="18"/>
-      <c r="AM4" s="18"/>
-    </row>
-    <row r="5" spans="1:39" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+    </row>
+    <row r="5" spans="1:40" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>72</v>
       </c>
@@ -1502,7 +1523,7 @@
         <v>92</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="W5" s="9" t="s">
         <v>93</v>
@@ -1535,28 +1556,31 @@
         <v>102</v>
       </c>
       <c r="AG5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AI5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="AI5" s="9" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="AJ5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AL5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="AL5" s="9" t="s">
+      <c r="AM5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AM5" s="9" t="s">
+      <c r="AN5" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1622,13 +1646,13 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W6" s="12">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X6" s="12">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
         <v>115</v>
@@ -1654,31 +1678,34 @@
       <c r="AF6" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH6">
         <v>200</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AI6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>120</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>10</v>
       </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AL6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>200</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>111</v>
@@ -1741,11 +1768,11 @@
       <c r="U7" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V7" s="25" t="s">
-        <v>163</v>
+      <c r="V7" s="26" t="s">
+        <v>161</v>
       </c>
       <c r="W7" s="12">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X7" s="12">
         <v>0.12</v>
@@ -1774,41 +1801,62 @@
       <c r="AF7" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH7">
         <v>200</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AI7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>120</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>10</v>
       </c>
-      <c r="AK7" s="2" t="s">
+      <c r="AL7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>200</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C8" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
       <c r="J8" s="12">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K8" s="13" t="b">
         <v>1</v>
@@ -1841,11 +1889,17 @@
         <v>0.01</v>
       </c>
       <c r="U8" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="W8" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X8" s="12">
+        <v>0</v>
+      </c>
       <c r="Y8" t="s">
         <v>115</v>
       </c>
@@ -1870,19 +1924,28 @@
       <c r="AF8" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH8">
         <v>200</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AI8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AK8" s="2" t="s">
+      <c r="AJ8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK8">
+        <v>10</v>
+      </c>
+      <c r="AL8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>200</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>1</v>
       </c>
     </row>
@@ -1893,8 +1956,8 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AM4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AJ4:AN4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
@@ -1902,11 +1965,11 @@
     <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI8">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL8">
       <formula1>"MA,AL"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1922,7 +1985,7 @@
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K8 C6:C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C8 K6:K8">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1930,7 +1993,7 @@
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T8 P6:P8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P8 T6:T8">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
@@ -1938,7 +2001,7 @@
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V8 W6:W8 U6:U8 S6:S8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S8 U6:U8 W6:W8">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
@@ -1958,19 +2021,19 @@
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AJ6:AJ8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK8">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM8">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM8">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN8">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V8"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="V7" r:id="rId1" location="Returns!A1"/>
@@ -1982,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D7"/>
+  <dimension ref="A3:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,93 +2064,124 @@
         <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B4" s="12">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C4" s="12">
         <v>0.12</v>
       </c>
       <c r="D4">
-        <v>105</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C5" s="12">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B6" s="12">
-        <v>5.5E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C6" s="12">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0</v>
-      </c>
-      <c r="D7">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="C4:C7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="C4:C6">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B6">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>GlobalParams!A3</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="27">
+        <v>11</v>
+      </c>
+      <c r="C3" s="27">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="27">
+        <v>20</v>
+      </c>
+      <c r="C4" s="27">
+        <v>4</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2102,30 +2196,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2157,7 +2251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
@@ -2175,7 +2269,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2185,15 +2279,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2206,23 +2300,23 @@
         <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2235,23 +2329,23 @@
         <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2264,15 +2358,15 @@
         <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2285,15 +2379,15 @@
         <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2306,15 +2400,15 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2327,15 +2421,15 @@
         <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2348,15 +2442,15 @@
         <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2369,31 +2463,31 @@
         <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2406,7 +2500,7 @@
         <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>